<commit_message>
Added update deviceProfile functionality
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamil\Documents\Visual Studio 2019\Projects\gps_loader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C929E2D1-EB09-4E0D-AC41-1924F0D0C00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D6645C-87BA-4BCD-BEF1-140E5FC58A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8340" yWindow="1665" windowWidth="13740" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>devEui</t>
   </si>
@@ -79,6 +79,15 @@
   </si>
   <si>
     <t>value _3n…</t>
+  </si>
+  <si>
+    <t>deviceProfileId</t>
+  </si>
+  <si>
+    <t>ddf28dd5-093e-4657-9a6d-b5b49904f942</t>
+  </si>
+  <si>
+    <t>b0dac1ac-3234-44d3-b290-59b7f5803300</t>
   </si>
 </sst>
 </file>
@@ -397,110 +406,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="40.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
         <v>51.104475770000001</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>17.0470431</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>5167785</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3">
         <v>51.104456730000003</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>17.047089400000001</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>6463345</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
         <v>51.107456749999997</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>17.0370332</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2131231</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>